<commit_message>
Changed stimuli colours to not conflict with AR task
</commit_message>
<xml_diff>
--- a/Exp1Conditions.xlsx
+++ b/Exp1Conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Python Scripts\PsychoPy Experiments\Experiment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD918A37-B598-4C07-840C-96EFCFF43F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A09BA2-C342-4793-9A21-9475A88CFDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26160" yWindow="-810" windowWidth="13485" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1560" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>cue_file</t>
-  </si>
-  <si>
-    <t>images/GoIcon.png</t>
   </si>
   <si>
     <t>images/StopIcon.png</t>
   </si>
   <si>
     <t>position</t>
+  </si>
+  <si>
+    <t>images/YellowIcon.png</t>
+  </si>
+  <si>
+    <t>images/OrangeIcon.png</t>
   </si>
 </sst>
 </file>
@@ -354,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -370,12 +373,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>0.5</v>
@@ -383,7 +386,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>-0.5</v>
@@ -391,7 +394,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -399,9 +402,25 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
         <v>-0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added sound and sorted RBG profile of images
</commit_message>
<xml_diff>
--- a/Exp1Conditions.xlsx
+++ b/Exp1Conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Python Scripts\PsychoPy Experiments\Experiment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\OneDrive - University of Glasgow\Documents\Python Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A09BA2-C342-4793-9A21-9475A88CFDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53459179-2ED6-4F54-9C6E-19F2FE3D936F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1560" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="864" yWindow="864" windowWidth="17280" windowHeight="8946" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,12 +363,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -376,7 +376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -384,7 +384,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -392,7 +392,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -400,7 +400,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -408,7 +408,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -416,7 +416,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Added practice routine - need to add feedback
</commit_message>
<xml_diff>
--- a/Exp1Conditions.xlsx
+++ b/Exp1Conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\OneDrive - University of Glasgow\Documents\Python Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53459179-2ED6-4F54-9C6E-19F2FE3D936F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9AFEDC-C253-42CC-856A-780C83A887DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="864" yWindow="864" windowWidth="17280" windowHeight="8946" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>cue_file</t>
   </si>
@@ -33,13 +33,19 @@
     <t>images/StopIcon.png</t>
   </si>
   <si>
-    <t>position</t>
-  </si>
-  <si>
     <t>images/YellowIcon.png</t>
   </si>
   <si>
     <t>images/OrangeIcon.png</t>
+  </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
+  </si>
+  <si>
+    <t>Correct</t>
   </si>
 </sst>
 </file>
@@ -357,71 +363,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>-0.5</v>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>-0.5</v>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added feedback images - needs testing
</commit_message>
<xml_diff>
--- a/Exp1Conditions.xlsx
+++ b/Exp1Conditions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\OneDrive - University of Glasgow\Documents\Python Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Python Scripts\PsychoPy Experiments\Experiment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9AFEDC-C253-42CC-856A-780C83A887DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B870BD-FDA8-4D01-B2A7-E58CDC38DE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26160" yWindow="-810" windowWidth="13485" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,10 +42,10 @@
     <t>response</t>
   </si>
   <si>
-    <t>Incorrect</t>
-  </si>
-  <si>
-    <t>Correct</t>
+    <t>images/Incorrect.png</t>
+  </si>
+  <si>
+    <t>images/Correct.png</t>
   </si>
 </sst>
 </file>
@@ -366,15 +366,15 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -390,7 +390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -398,7 +398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Added conditional feedback trials
</commit_message>
<xml_diff>
--- a/Exp1Conditions.xlsx
+++ b/Exp1Conditions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Python Scripts\PsychoPy Experiments\Experiment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\OneDrive - University of Glasgow\Documents\Python Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B870BD-FDA8-4D01-B2A7-E58CDC38DE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38E7403-3A62-497E-8265-0FAC7F0226E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26160" yWindow="-810" windowWidth="13485" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>cue_file</t>
   </si>
@@ -39,13 +39,10 @@
     <t>images/OrangeIcon.png</t>
   </si>
   <si>
-    <t>response</t>
-  </si>
-  <si>
-    <t>images/Incorrect.png</t>
-  </si>
-  <si>
-    <t>images/Correct.png</t>
+    <t>space</t>
+  </si>
+  <si>
+    <t>corrAns</t>
   </si>
 </sst>
 </file>
@@ -366,44 +363,39 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>